<commit_message>
Added share dilution to DCF models. Added ZI, MCO, SPGI, MSCI, AMD models
</commit_message>
<xml_diff>
--- a/Technology/ASML.xlsx
+++ b/Technology/ASML.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Growth Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Technology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE25ACF-F22E-A846-B3BF-EED42346C88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260057D7-555F-2D4C-A0E6-586163113CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28460" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="162">
   <si>
     <t>INCOME STATEMENT (in mln.)</t>
   </si>
@@ -516,6 +516,9 @@
   </si>
   <si>
     <t>P/FCF</t>
+  </si>
+  <si>
+    <t>Net Cash</t>
   </si>
 </sst>
 </file>
@@ -858,7 +861,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -949,7 +952,6 @@
     <xf numFmtId="164" fontId="1" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1000,6 +1002,15 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2593,10 +2604,10 @@
   <dimension ref="A1:AL119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="W80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AI26" sqref="AI26"/>
+      <selection pane="bottomRight" activeCell="AF86" sqref="AF86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2971,13 +2982,13 @@
       <c r="AH4" s="25">
         <v>45895000000</v>
       </c>
-      <c r="AI4" s="57" t="s">
+      <c r="AI4" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="AJ4" s="57" t="s">
+      <c r="AJ4" s="56" t="s">
         <v>110</v>
       </c>
-      <c r="AK4" s="57" t="s">
+      <c r="AK4" s="56" t="s">
         <v>111</v>
       </c>
       <c r="AL4" s="18" t="s">
@@ -3117,15 +3128,15 @@
         <f t="shared" si="9"/>
         <v>0.11827197193050853</v>
       </c>
-      <c r="AI5" s="58">
+      <c r="AI5" s="57">
         <f>(AC5+AB5+AA5)/3</f>
         <v>0.21723267494156651</v>
       </c>
-      <c r="AJ5" s="58">
+      <c r="AJ5" s="57">
         <f>(AC21+AB21+AA21)/3</f>
         <v>0.32336582629238492</v>
       </c>
-      <c r="AK5" s="58">
+      <c r="AK5" s="57">
         <f>(AC30+AB30+AA30)/3</f>
         <v>0.32286462810370614</v>
       </c>
@@ -3311,13 +3322,13 @@
       <c r="AC7" s="10">
         <v>10700100000</v>
       </c>
-      <c r="AI7" s="57" t="s">
+      <c r="AI7" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="AJ7" s="57" t="s">
+      <c r="AJ7" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="AK7" s="57" t="s">
+      <c r="AK7" s="56" t="s">
         <v>115</v>
       </c>
       <c r="AL7" s="18" t="s">
@@ -3412,15 +3423,15 @@
       <c r="AC8" s="2">
         <v>0.50539999999999996</v>
       </c>
-      <c r="AI8" s="58">
+      <c r="AI8" s="57">
         <f>AC8</f>
         <v>0.50539999999999996</v>
       </c>
-      <c r="AJ8" s="58">
+      <c r="AJ8" s="57">
         <f>AC22</f>
         <v>0.33040000000000003</v>
       </c>
-      <c r="AK8" s="58">
+      <c r="AK8" s="57">
         <f>AC31</f>
         <v>0.2591</v>
       </c>
@@ -3634,7 +3645,7 @@
         <f t="shared" ref="AC10" si="22">AC9/AC4</f>
         <v>0.15365978066819688</v>
       </c>
-      <c r="AI10" s="57" t="s">
+      <c r="AI10" s="56" t="s">
         <v>97</v>
       </c>
       <c r="AJ10" s="18" t="s">
@@ -3735,15 +3746,15 @@
       <c r="AC11" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AI11" s="58">
+      <c r="AI11" s="57">
         <f>(AC10+AB10+AA10)/3</f>
         <v>0.14931870488429119</v>
       </c>
-      <c r="AJ11" s="58">
+      <c r="AJ11" s="57">
         <f>(AC14+AB14+AA14)/3</f>
         <v>4.0880988625067081E-2</v>
       </c>
-      <c r="AK11" s="58">
+      <c r="AK11" s="57">
         <f>(AC81+AB81+AA81)/3</f>
         <v>4.4744916917326275E-3</v>
       </c>
@@ -3929,13 +3940,13 @@
       <c r="AC13" s="1">
         <v>945900000</v>
       </c>
-      <c r="AI13" s="57" t="s">
+      <c r="AI13" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="AJ13" s="57" t="s">
+      <c r="AJ13" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="AK13" s="57" t="s">
+      <c r="AK13" s="56" t="s">
         <v>119</v>
       </c>
       <c r="AL13" s="18" t="s">
@@ -4058,7 +4069,7 @@
         <f t="shared" ref="AC14" si="35">AC13/AC4</f>
         <v>4.4673977726770384E-2</v>
       </c>
-      <c r="AI14" s="58">
+      <c r="AI14" s="57">
         <f>AC29/AC73</f>
         <v>0.62266763517501245</v>
       </c>
@@ -4066,7 +4077,7 @@
         <f>AC29/AC55</f>
         <v>0.15113332084494938</v>
       </c>
-      <c r="AK14" s="58">
+      <c r="AK14" s="57">
         <f>(AC29-AC99)/AC74</f>
         <v>0.2216504501327809</v>
       </c>
@@ -4252,7 +4263,7 @@
       <c r="AC16" s="1">
         <v>4199400000</v>
       </c>
-      <c r="AI16" s="57" t="s">
+      <c r="AI16" s="56" t="s">
         <v>141</v>
       </c>
       <c r="AJ16" s="18" t="s">
@@ -4261,7 +4272,7 @@
       <c r="AK16" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="AL16" s="59" t="s">
+      <c r="AL16" s="58" t="s">
         <v>160</v>
       </c>
     </row>
@@ -4357,15 +4368,15 @@
         <f>(SUM(Y36:AC36)/5)</f>
         <v>-9.9987576959951977E-3</v>
       </c>
-      <c r="AJ17" s="60">
+      <c r="AJ17" s="59">
         <f>AK101/AC4</f>
         <v>11.712809468484041</v>
       </c>
-      <c r="AK17" s="60">
+      <c r="AK17" s="59">
         <f>AK101/AC26</f>
         <v>38.41328356128313</v>
       </c>
-      <c r="AL17" s="61">
+      <c r="AL17" s="60">
         <f>AK101/AC107</f>
         <v>34.600627833972794</v>
       </c>
@@ -4459,7 +4470,7 @@
         <v>-44600000</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" ht="20" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>13</v>
       </c>
@@ -4546,6 +4557,9 @@
       </c>
       <c r="AC19" s="1">
         <v>583600000</v>
+      </c>
+      <c r="AI19" s="69" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:38" ht="19" x14ac:dyDescent="0.25">
@@ -4636,6 +4650,10 @@
       <c r="AC20" s="10">
         <v>6995100000</v>
       </c>
+      <c r="AI20" s="70">
+        <f>AC41-AC57-AC62</f>
+        <v>3861800000</v>
+      </c>
     </row>
     <row r="21" spans="1:38" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
@@ -10346,10 +10364,10 @@
       <c r="AC83" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AJ83" s="68" t="s">
+      <c r="AJ83" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="AK83" s="69"/>
+      <c r="AK83" s="68"/>
     </row>
     <row r="84" spans="1:37" ht="19" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
@@ -10439,10 +10457,10 @@
       <c r="AC84" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AJ84" s="62" t="s">
+      <c r="AJ84" s="61" t="s">
         <v>122</v>
       </c>
-      <c r="AK84" s="63"/>
+      <c r="AK84" s="62"/>
     </row>
     <row r="85" spans="1:37" ht="20" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
@@ -11328,10 +11346,10 @@
       <c r="AC93" s="1">
         <v>864700000</v>
       </c>
-      <c r="AJ93" s="62" t="s">
+      <c r="AJ93" s="61" t="s">
         <v>129</v>
       </c>
-      <c r="AK93" s="63"/>
+      <c r="AK93" s="62"/>
     </row>
     <row r="94" spans="1:37" ht="20" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
@@ -11802,10 +11820,10 @@
       <c r="AC98" s="1">
         <v>-4639700000</v>
       </c>
-      <c r="AJ98" s="62" t="s">
+      <c r="AJ98" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="AK98" s="63"/>
+      <c r="AK98" s="62"/>
     </row>
     <row r="99" spans="1:37" ht="20" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
@@ -12374,10 +12392,10 @@
       <c r="AC104" s="1">
         <v>6951800000</v>
       </c>
-      <c r="AJ104" s="62" t="s">
+      <c r="AJ104" s="61" t="s">
         <v>139</v>
       </c>
-      <c r="AK104" s="63"/>
+      <c r="AK104" s="62"/>
     </row>
     <row r="105" spans="1:37" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="7" t="s">
@@ -12594,10 +12612,10 @@
       <c r="AG106" s="15"/>
       <c r="AH106" s="15"/>
       <c r="AI106" s="15"/>
-      <c r="AJ106" s="64" t="s">
+      <c r="AJ106" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="AK106" s="65"/>
+      <c r="AK106" s="64"/>
     </row>
     <row r="107" spans="1:37" ht="19" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
@@ -12770,10 +12788,10 @@
       </c>
     </row>
     <row r="110" spans="1:37" ht="19" x14ac:dyDescent="0.25">
-      <c r="AD110" s="66" t="s">
+      <c r="AD110" s="65" t="s">
         <v>149</v>
       </c>
-      <c r="AE110" s="67"/>
+      <c r="AE110" s="66"/>
     </row>
     <row r="111" spans="1:37" ht="20" x14ac:dyDescent="0.25">
       <c r="AD111" s="47" t="s">
@@ -12812,44 +12830,45 @@
       </c>
     </row>
     <row r="115" spans="30:31" ht="20" x14ac:dyDescent="0.25">
-      <c r="AD115" s="49" t="s">
+      <c r="AD115" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="AE115" s="50">
-        <v>394590000</v>
+      <c r="AE115" s="71">
+        <f>AC35*(1+(5*AI17))</f>
+        <v>389882549.20781785</v>
       </c>
     </row>
     <row r="116" spans="30:31" ht="20" x14ac:dyDescent="0.25">
-      <c r="AD116" s="51" t="s">
+      <c r="AD116" s="50" t="s">
         <v>154</v>
       </c>
-      <c r="AE116" s="52">
+      <c r="AE116" s="51">
         <f>AE114/AE115</f>
-        <v>510.65022376259236</v>
+        <v>516.81582621200562</v>
       </c>
     </row>
     <row r="117" spans="30:31" ht="20" x14ac:dyDescent="0.25">
       <c r="AD117" s="49" t="s">
         <v>155</v>
       </c>
-      <c r="AE117" s="53">
+      <c r="AE117" s="52">
         <v>609.11</v>
       </c>
     </row>
     <row r="118" spans="30:31" ht="20" x14ac:dyDescent="0.25">
-      <c r="AD118" s="54" t="s">
+      <c r="AD118" s="53" t="s">
         <v>156</v>
       </c>
-      <c r="AE118" s="55">
+      <c r="AE118" s="54">
         <f>AE116/AE117-1</f>
-        <v>-0.16164531240237012</v>
+        <v>-0.15152299878182007</v>
       </c>
     </row>
     <row r="119" spans="30:31" ht="20" x14ac:dyDescent="0.25">
-      <c r="AD119" s="54" t="s">
+      <c r="AD119" s="53" t="s">
         <v>157</v>
       </c>
-      <c r="AE119" s="56" t="str">
+      <c r="AE119" s="55" t="str">
         <f>IF(AE116&gt;AE117,"BUY","SELL")</f>
         <v>SELL</v>
       </c>

</xml_diff>